<commit_message>
Fixed errors. All tests pass. Partner.
</commit_message>
<xml_diff>
--- a/MBSR_ClueDesign.xlsx
+++ b/MBSR_ClueDesign.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306WS\ClueGameMBSR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306WS\ClueGameMBTS\ClueGameMBTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="46">
   <si>
     <t>M</t>
   </si>
@@ -127,6 +127,36 @@
   </si>
   <si>
     <t>Number of Doors: 29</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>KN</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>DN</t>
+  </si>
+  <si>
+    <t>LN</t>
+  </si>
+  <si>
+    <t>VN</t>
   </si>
 </sst>
 </file>
@@ -645,7 +675,7 @@
   <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -729,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -747,7 +777,7 @@
         <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>3</v>
@@ -851,7 +881,7 @@
         <v>4</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>4</v>
@@ -1117,7 +1147,7 @@
         <v>15</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="I7" s="30" t="s">
         <v>15</v>
@@ -1173,7 +1203,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
@@ -1591,7 +1621,7 @@
         <v>16</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>16</v>
@@ -1617,7 +1647,7 @@
         <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>19</v>
@@ -1632,7 +1662,7 @@
         <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>14</v>
@@ -2061,7 +2091,7 @@
         <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>24</v>
@@ -2091,7 +2121,7 @@
         <v>11</v>
       </c>
       <c r="L20" s="29" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="M20" s="29" t="s">
         <v>11</v>

</xml_diff>